<commit_message>
Added zoom , maze regenerate and set wallheight functions
</commit_message>
<xml_diff>
--- a/Documents/DTT-Assessment-Hour-Log .xlsx
+++ b/Documents/DTT-Assessment-Hour-Log .xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26105"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1649045B-160E-4E8C-B1AD-241B9FBC519D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B7802448-DCE0-4800-999B-E626224234EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Uur</t>
   </si>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t>Ik heb de ontwikkelontgeving opgezet in Unity, een git repo gemaakt en het algoritme voor de maze generation geschreven. Hiervoor heb ik een tutorial gevolgd. Deze is gelinked in het bijgeleverde README bestand.</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>In dit uur heb ik een in en uit zoom functie script gemaakt voor de camera. Zo kan de user makkelijker de hele maze zien. Daarna heb ik de code geschreven om de hoogte van de muren te kunen instellen. Als laatste heb ik ervoor gezorgd dat de user een nieuwe maze kan generaten door op "G" te drukken. De oude maze word hierdoor verwijderd en daarna word de nieuwe gemaakt.</t>
   </si>
 </sst>
 </file>
@@ -412,16 +418,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="194.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="255.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -447,6 +453,17 @@
         <v>4</v>
       </c>
     </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>